<commit_message>
Actualizacion de errores, mantenimiento medida mitigacion
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico/MRVMinem/Documentos/1.3 Plantilla_Eficiencia_energetica_comercial.xlsx
+++ b/back-end/Web Dinamico/MRVMinem/Documentos/1.3 Plantilla_Eficiencia_energetica_comercial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\ALFREDO\Archivos Compu DELL\Escritorio\MRV MINEM 1.0 Tercer Entregable-Mantenimientos\Enfoque excel\Enfoque Eficiencia energetica comercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C19177B-BAF8-41EC-A8E1-D31F009BFCAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DFDE62-E100-471E-B845-115571375213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{71D78059-0FA9-459A-8548-6759DAA3D3F6}"/>
   </bookViews>
@@ -722,7 +722,7 @@
   <dimension ref="A1:F310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>